<commit_message>
Spring 1: HU2: Informe de avance
</commit_message>
<xml_diff>
--- a/CRONOGRAMA/Springs.xlsx
+++ b/CRONOGRAMA/Springs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danki\Documents\universidad\taller-proyectos-1\CRONOGRAMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7E53A53-D6ED-4A7C-B191-6E0EC40C5513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A058B4-9F4F-42D2-BD22-E277CA155BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{EF0BB044-1F90-41AD-8557-97E247B6327D}"/>
   </bookViews>
@@ -248,13 +248,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -264,6 +257,13 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -354,13 +354,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -370,6 +363,13 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -460,13 +460,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -476,6 +469,13 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -525,18 +525,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -578,13 +566,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -597,6 +578,25 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -802,6 +802,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4980,10 +4998,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A27258C-A107-40C2-88F9-5F0E9320079F}" name="Tabla1" displayName="Tabla1" ref="A1:C7" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="22" tableBorderDxfId="23" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A27258C-A107-40C2-88F9-5F0E9320079F}" name="Tabla1" displayName="Tabla1" ref="A1:C7" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="A1:C7" xr:uid="{7A27258C-A107-40C2-88F9-5F0E9320079F}"/>
   <tableColumns count="3">
-    <tableColumn id="2" xr3:uid="{BF8E4A42-83BA-4EC3-9E35-814F42DE5ABE}" name="Tiempo" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{BF8E4A42-83BA-4EC3-9E35-814F42DE5ABE}" name="Tiempo" dataDxfId="19"/>
     <tableColumn id="3" xr3:uid="{0D3743C7-30C2-4060-9F35-A1C94C62C878}" name="Actividad" dataDxfId="18"/>
     <tableColumn id="4" xr3:uid="{09F1400E-2329-4B27-805C-C84709A4E2AD}" name="Avance"/>
   </tableColumns>
@@ -4992,7 +5010,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{660D6E44-310E-40FA-9E2C-F462D7E6840E}" name="Tabla13" displayName="Tabla13" ref="A1:C7" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{660D6E44-310E-40FA-9E2C-F462D7E6840E}" name="Tabla13" displayName="Tabla13" ref="A1:C7" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A1:C7" xr:uid="{7A27258C-A107-40C2-88F9-5F0E9320079F}"/>
   <tableColumns count="3">
     <tableColumn id="2" xr3:uid="{094294A4-DF14-4F30-BB67-F28A7A930213}" name="Tiempo" dataDxfId="13"/>
@@ -5004,7 +5022,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{422867AE-C70C-46E3-BA50-6A64183CCAAD}" name="Tabla134" displayName="Tabla134" ref="A1:C6" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{422867AE-C70C-46E3-BA50-6A64183CCAAD}" name="Tabla134" displayName="Tabla134" ref="A1:C6" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A1:C6" xr:uid="{7A27258C-A107-40C2-88F9-5F0E9320079F}"/>
   <tableColumns count="3">
     <tableColumn id="2" xr3:uid="{38524CCE-A412-49EA-A1DF-935EFC9F0B19}" name="Tiempo" dataDxfId="7"/>
@@ -5016,7 +5034,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{33D0E118-132A-4FC4-82EF-3325C90AEFA6}" name="Tabla1345" displayName="Tabla1345" ref="A1:C5" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{33D0E118-132A-4FC4-82EF-3325C90AEFA6}" name="Tabla1345" displayName="Tabla1345" ref="A1:C5" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="A1:C5" xr:uid="{7A27258C-A107-40C2-88F9-5F0E9320079F}"/>
   <tableColumns count="3">
     <tableColumn id="2" xr3:uid="{1E950689-A2DA-4380-A44A-BE1EF295CB9E}" name="Tiempo" dataDxfId="1"/>
@@ -5347,7 +5365,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5370,6 +5388,9 @@
       <c r="B2" s="1">
         <v>5</v>
       </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
       <c r="D2" s="6">
         <v>6.4</v>
       </c>
@@ -5382,6 +5403,9 @@
       <c r="B3" s="1">
         <v>4</v>
       </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -5391,6 +5415,9 @@
       <c r="B4" s="1">
         <v>3</v>
       </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -5400,6 +5427,9 @@
       <c r="B5" s="1">
         <v>2</v>
       </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -5409,6 +5439,9 @@
       <c r="B6" s="4">
         <v>1</v>
       </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -5416,6 +5449,9 @@
         <v>32</v>
       </c>
       <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Spring 2: HU3: Diseño de interfaz de imagenes y mapas del sitios turistico
</commit_message>
<xml_diff>
--- a/CRONOGRAMA/Springs.xlsx
+++ b/CRONOGRAMA/Springs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1" sheetId="1" state="visible" r:id="rId3"/>
@@ -98,7 +98,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -141,6 +141,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -167,33 +174,45 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -559,11 +578,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="24905512"/>
-        <c:axId val="47039914"/>
+        <c:axId val="24060554"/>
+        <c:axId val="7444029"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="24905512"/>
+        <c:axId val="24060554"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,7 +648,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47039914"/>
+        <c:crossAx val="7444029"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -637,7 +656,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47039914"/>
+        <c:axId val="7444029"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -710,7 +729,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24905512"/>
+        <c:crossAx val="24060554"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1006,6 +1025,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1019,11 +1056,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="68436792"/>
-        <c:axId val="17878819"/>
+        <c:axId val="15669978"/>
+        <c:axId val="68179411"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68436792"/>
+        <c:axId val="15669978"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1089,7 +1126,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17878819"/>
+        <c:crossAx val="68179411"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1097,7 +1134,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="17878819"/>
+        <c:axId val="68179411"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1170,7 +1207,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68436792"/>
+        <c:crossAx val="15669978"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1470,11 +1507,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="78277523"/>
-        <c:axId val="38018401"/>
+        <c:axId val="41514734"/>
+        <c:axId val="96301378"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78277523"/>
+        <c:axId val="41514734"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1540,7 +1577,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38018401"/>
+        <c:crossAx val="96301378"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1548,7 +1585,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38018401"/>
+        <c:axId val="96301378"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1621,7 +1658,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78277523"/>
+        <c:crossAx val="41514734"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1912,11 +1949,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="73457007"/>
-        <c:axId val="11669557"/>
+        <c:axId val="60665670"/>
+        <c:axId val="85763478"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73457007"/>
+        <c:axId val="60665670"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1982,7 +2019,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11669557"/>
+        <c:crossAx val="85763478"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1990,7 +2027,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11669557"/>
+        <c:axId val="85763478"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2063,7 +2100,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73457007"/>
+        <c:crossAx val="60665670"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2127,9 +2164,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>180720</xdr:colOff>
+      <xdr:colOff>180360</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2138,7 +2175,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3927600" y="662040"/>
-        <a:ext cx="5619240" cy="2742840"/>
+        <a:ext cx="5618880" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2162,9 +2199,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>180720</xdr:colOff>
+      <xdr:colOff>180360</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2173,7 +2210,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3927600" y="662040"/>
-        <a:ext cx="5619240" cy="2742840"/>
+        <a:ext cx="5618880" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2197,9 +2234,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>180720</xdr:colOff>
+      <xdr:colOff>180360</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2208,7 +2245,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3927600" y="662040"/>
-        <a:ext cx="5619240" cy="2552400"/>
+        <a:ext cx="5618880" cy="2552040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2232,9 +2269,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>180720</xdr:colOff>
+      <xdr:colOff>180360</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2243,7 +2280,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3927600" y="662040"/>
-        <a:ext cx="5619240" cy="2361960"/>
+        <a:ext cx="5618880" cy="2361600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2479,8 +2516,8 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2503,10 +2540,10 @@
       <c r="B2" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="D2" s="6" t="n">
         <v>6.4</v>
       </c>
     </row>
@@ -2518,7 +2555,7 @@
       <c r="B3" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="5" t="n">
         <v>4</v>
       </c>
     </row>
@@ -2530,7 +2567,7 @@
       <c r="B4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="5" t="n">
         <v>4</v>
       </c>
     </row>
@@ -2542,7 +2579,7 @@
       <c r="B5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="5" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2551,10 +2588,10 @@
         <f aca="false">A5+$D$2</f>
         <v>25.6</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="5" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2563,10 +2600,10 @@
         <f aca="false">A6+$D$2</f>
         <v>32</v>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B7" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2592,8 +2629,8 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2610,59 +2647,77 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="C2" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6" t="n">
         <v>6.4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="8" t="n">
         <f aca="false">A2+$D$2</f>
         <v>6.4</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="8" t="n">
         <v>4</v>
+      </c>
+      <c r="C3" s="9" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="8" t="n">
         <f aca="false">A3+$D$2</f>
         <v>12.8</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="8" t="n">
         <v>3</v>
+      </c>
+      <c r="C4" s="9" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="8" t="n">
         <f aca="false">A4+$D$2</f>
         <v>19.2</v>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="8" t="n">
         <v>2</v>
+      </c>
+      <c r="C5" s="9" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="8" t="n">
         <f aca="false">A5+$D$2</f>
         <v>25.6</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="8" t="n">
         <v>1</v>
+      </c>
+      <c r="C6" s="9" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+      <c r="A7" s="8" t="n">
         <f aca="false">A6+$D$2</f>
         <v>32</v>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B7" s="8" t="n">
         <v>0</v>
+      </c>
+      <c r="C7" s="9" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2711,7 +2766,7 @@
       <c r="B2" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="D2" s="6" t="n">
         <v>6.4</v>
       </c>
     </row>
@@ -2743,7 +2798,7 @@
       <c r="A6" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2793,7 +2848,7 @@
       <c r="B2" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="D2" s="6" t="n">
         <v>6.4</v>
       </c>
     </row>

</xml_diff>